<commit_message>
Docs according FW rev. 67
</commit_message>
<xml_diff>
--- a/MG996R calibration tables.xlsx
+++ b/MG996R calibration tables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="MG996R #6" sheetId="8" r:id="rId7"/>
     <sheet name="DS3218MG #7-#18" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -574,59 +574,20 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -697,9 +658,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -712,9 +712,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -752,7 +752,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -824,7 +824,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1001,8 +1001,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,78 +1013,78 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28"/>
-      <c r="C3" s="29">
+      <c r="B3" s="42"/>
+      <c r="C3" s="16">
         <v>1</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="17">
         <v>2</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="17">
         <v>3</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="17">
         <v>4</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="17">
         <v>5</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="18">
         <v>6</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="50">
+      <c r="B4" s="37">
         <v>0</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="33">
+        <v>750</v>
+      </c>
+      <c r="D4" s="23">
+        <v>640</v>
+      </c>
+      <c r="E4" s="23">
+        <v>610</v>
+      </c>
+      <c r="F4" s="23">
         <v>580</v>
       </c>
-      <c r="D4" s="36">
-        <v>640</v>
-      </c>
-      <c r="E4" s="36">
+      <c r="G4" s="23">
         <v>610</v>
       </c>
-      <c r="F4" s="36">
+      <c r="H4" s="25">
         <v>580</v>
       </c>
-      <c r="G4" s="36">
-        <v>610</v>
-      </c>
-      <c r="H4" s="38">
-        <v>580</v>
-      </c>
-      <c r="I4" s="43">
+      <c r="I4" s="30">
         <f>ROUND(500 +( (2500 - 500) / 270 * B4), 0)</f>
         <v>500</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="51">
+      <c r="B5" s="38">
         <v>10</v>
       </c>
-      <c r="C5" s="47">
-        <v>665</v>
+      <c r="C5" s="34">
+        <v>830</v>
       </c>
       <c r="D5" s="3">
         <v>730</v>
@@ -1098,20 +1098,20 @@
       <c r="G5" s="3">
         <v>680</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="26">
         <v>660</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="31">
         <f t="shared" ref="I5:I31" si="0">ROUND(500 +( (2500 - 500) / 270 * B5), 0)</f>
         <v>574</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="51">
+      <c r="B6" s="38">
         <v>20</v>
       </c>
-      <c r="C6" s="47">
-        <v>750</v>
+      <c r="C6" s="34">
+        <v>930</v>
       </c>
       <c r="D6" s="3">
         <v>800</v>
@@ -1125,20 +1125,20 @@
       <c r="G6" s="3">
         <v>750</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="26">
         <v>750</v>
       </c>
-      <c r="I6" s="44">
+      <c r="I6" s="31">
         <f t="shared" si="0"/>
         <v>648</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="51">
+      <c r="B7" s="38">
         <v>30</v>
       </c>
-      <c r="C7" s="47">
-        <v>830</v>
+      <c r="C7" s="34">
+        <v>1000</v>
       </c>
       <c r="D7" s="3">
         <v>890</v>
@@ -1152,20 +1152,20 @@
       <c r="G7" s="3">
         <v>830</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="26">
         <v>830</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="31">
         <f t="shared" si="0"/>
         <v>722</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="51">
+      <c r="B8" s="38">
         <v>40</v>
       </c>
-      <c r="C8" s="47">
-        <v>915</v>
+      <c r="C8" s="34">
+        <v>1080</v>
       </c>
       <c r="D8" s="3">
         <v>985</v>
@@ -1179,20 +1179,20 @@
       <c r="G8" s="3">
         <v>910</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="26">
         <v>915</v>
       </c>
-      <c r="I8" s="44">
+      <c r="I8" s="31">
         <f t="shared" si="0"/>
         <v>796</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="51">
+      <c r="B9" s="38">
         <v>50</v>
       </c>
-      <c r="C9" s="47">
-        <v>990</v>
+      <c r="C9" s="34">
+        <v>1180</v>
       </c>
       <c r="D9" s="3">
         <v>1070</v>
@@ -1206,20 +1206,20 @@
       <c r="G9" s="3">
         <v>990</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="26">
         <v>990</v>
       </c>
-      <c r="I9" s="44">
+      <c r="I9" s="31">
         <f t="shared" si="0"/>
         <v>870</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="51">
+      <c r="B10" s="38">
         <v>60</v>
       </c>
-      <c r="C10" s="47">
-        <v>1070</v>
+      <c r="C10" s="34">
+        <v>1250</v>
       </c>
       <c r="D10" s="3">
         <v>1150</v>
@@ -1233,20 +1233,20 @@
       <c r="G10" s="3">
         <v>1070</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="26">
         <v>1070</v>
       </c>
-      <c r="I10" s="44">
+      <c r="I10" s="31">
         <f t="shared" si="0"/>
         <v>944</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="51">
+      <c r="B11" s="38">
         <v>70</v>
       </c>
-      <c r="C11" s="47">
-        <v>1160</v>
+      <c r="C11" s="34">
+        <v>1330</v>
       </c>
       <c r="D11" s="3">
         <v>1250</v>
@@ -1260,20 +1260,20 @@
       <c r="G11" s="3">
         <v>1160</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="26">
         <v>1160</v>
       </c>
-      <c r="I11" s="44">
+      <c r="I11" s="31">
         <f t="shared" si="0"/>
         <v>1019</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="51">
+      <c r="B12" s="38">
         <v>80</v>
       </c>
-      <c r="C12" s="47">
-        <v>1250</v>
+      <c r="C12" s="34">
+        <v>1420</v>
       </c>
       <c r="D12" s="3">
         <v>1340</v>
@@ -1287,47 +1287,47 @@
       <c r="G12" s="3">
         <v>1240</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="26">
         <v>1250</v>
       </c>
-      <c r="I12" s="44">
+      <c r="I12" s="31">
         <f t="shared" si="0"/>
         <v>1093</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="52">
+      <c r="B13" s="39">
         <v>90</v>
       </c>
-      <c r="C13" s="48">
-        <v>1350</v>
-      </c>
-      <c r="D13" s="33">
+      <c r="C13" s="35">
+        <v>1510</v>
+      </c>
+      <c r="D13" s="20">
         <v>1430</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="20">
         <v>1330</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="20">
         <v>1360</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="20">
         <v>1320</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="27">
         <v>1345</v>
       </c>
-      <c r="I13" s="44">
+      <c r="I13" s="31">
         <f t="shared" si="0"/>
         <v>1167</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="51">
+      <c r="B14" s="38">
         <v>100</v>
       </c>
-      <c r="C14" s="47">
-        <v>1450</v>
+      <c r="C14" s="34">
+        <v>1600</v>
       </c>
       <c r="D14" s="3">
         <v>1530</v>
@@ -1341,20 +1341,20 @@
       <c r="G14" s="3">
         <v>1400</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="26">
         <v>1440</v>
       </c>
-      <c r="I14" s="44">
+      <c r="I14" s="31">
         <f t="shared" si="0"/>
         <v>1241</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="51">
+      <c r="B15" s="38">
         <v>110</v>
       </c>
-      <c r="C15" s="47">
-        <v>1540</v>
+      <c r="C15" s="34">
+        <v>1690</v>
       </c>
       <c r="D15" s="3">
         <v>1620</v>
@@ -1368,20 +1368,20 @@
       <c r="G15" s="3">
         <v>1480</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="26">
         <v>1530</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="31">
         <f t="shared" si="0"/>
         <v>1315</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="51">
+      <c r="B16" s="38">
         <v>120</v>
       </c>
-      <c r="C16" s="47">
-        <v>1640</v>
+      <c r="C16" s="34">
+        <v>1780</v>
       </c>
       <c r="D16" s="3">
         <v>1710</v>
@@ -1395,20 +1395,20 @@
       <c r="G16" s="3">
         <v>1560</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="26">
         <v>1610</v>
       </c>
-      <c r="I16" s="44">
+      <c r="I16" s="31">
         <f t="shared" si="0"/>
         <v>1389</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="51">
+      <c r="B17" s="38">
         <v>130</v>
       </c>
-      <c r="C17" s="47">
-        <v>1740</v>
+      <c r="C17" s="34">
+        <v>1870</v>
       </c>
       <c r="D17" s="3">
         <v>1800</v>
@@ -1422,20 +1422,20 @@
       <c r="G17" s="3">
         <v>1640</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="26">
         <v>1690</v>
       </c>
-      <c r="I17" s="44">
+      <c r="I17" s="31">
         <f t="shared" si="0"/>
         <v>1463</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="51">
+      <c r="B18" s="38">
         <v>140</v>
       </c>
-      <c r="C18" s="47">
-        <v>1830</v>
+      <c r="C18" s="34">
+        <v>1960</v>
       </c>
       <c r="D18" s="3">
         <v>1900</v>
@@ -1449,20 +1449,20 @@
       <c r="G18" s="3">
         <v>1720</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="26">
         <v>1780</v>
       </c>
-      <c r="I18" s="44">
+      <c r="I18" s="31">
         <f t="shared" si="0"/>
         <v>1537</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="51">
+      <c r="B19" s="38">
         <v>150</v>
       </c>
-      <c r="C19" s="47">
-        <v>1920</v>
+      <c r="C19" s="34">
+        <v>2050</v>
       </c>
       <c r="D19" s="3">
         <v>1990</v>
@@ -1476,20 +1476,20 @@
       <c r="G19" s="3">
         <v>1800</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="26">
         <v>1860</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="31">
         <f t="shared" si="0"/>
         <v>1611</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="51">
+      <c r="B20" s="38">
         <v>160</v>
       </c>
-      <c r="C20" s="47">
-        <v>2010</v>
+      <c r="C20" s="34">
+        <v>2130</v>
       </c>
       <c r="D20" s="3">
         <v>2080</v>
@@ -1503,20 +1503,20 @@
       <c r="G20" s="3">
         <v>1900</v>
       </c>
-      <c r="H20" s="39">
+      <c r="H20" s="26">
         <v>1960</v>
       </c>
-      <c r="I20" s="44">
+      <c r="I20" s="31">
         <f t="shared" si="0"/>
         <v>1685</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="51">
+      <c r="B21" s="38">
         <v>170</v>
       </c>
-      <c r="C21" s="47">
-        <v>2105</v>
+      <c r="C21" s="34">
+        <v>2210</v>
       </c>
       <c r="D21" s="3">
         <v>2170</v>
@@ -1530,20 +1530,20 @@
       <c r="G21" s="3">
         <v>1970</v>
       </c>
-      <c r="H21" s="39">
+      <c r="H21" s="26">
         <v>2050</v>
       </c>
-      <c r="I21" s="44">
+      <c r="I21" s="31">
         <f t="shared" si="0"/>
         <v>1759</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="51">
+      <c r="B22" s="38">
         <v>180</v>
       </c>
-      <c r="C22" s="47">
-        <v>2200</v>
+      <c r="C22" s="34">
+        <v>2320</v>
       </c>
       <c r="D22" s="3">
         <v>2260</v>
@@ -1557,158 +1557,158 @@
       <c r="G22" s="3">
         <v>2070</v>
       </c>
-      <c r="H22" s="39">
+      <c r="H22" s="26">
         <v>2130</v>
       </c>
-      <c r="I22" s="44">
+      <c r="I22" s="31">
         <f t="shared" si="0"/>
         <v>1833</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="51">
+      <c r="B23" s="38">
         <v>190</v>
       </c>
-      <c r="C23" s="47"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="44">
+      <c r="H23" s="28"/>
+      <c r="I23" s="31">
         <f t="shared" si="0"/>
         <v>1907</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="51">
+      <c r="B24" s="38">
         <v>200</v>
       </c>
-      <c r="C24" s="47"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="44">
+      <c r="H24" s="28"/>
+      <c r="I24" s="31">
         <f t="shared" si="0"/>
         <v>1981</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="51">
+      <c r="B25" s="38">
         <v>210</v>
       </c>
-      <c r="C25" s="47"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="44">
+      <c r="H25" s="28"/>
+      <c r="I25" s="31">
         <f t="shared" si="0"/>
         <v>2056</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="51">
+      <c r="B26" s="38">
         <v>220</v>
       </c>
-      <c r="C26" s="47"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="44">
+      <c r="H26" s="28"/>
+      <c r="I26" s="31">
         <f t="shared" si="0"/>
         <v>2130</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="51">
+      <c r="B27" s="38">
         <v>230</v>
       </c>
-      <c r="C27" s="47"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="44">
+      <c r="H27" s="28"/>
+      <c r="I27" s="31">
         <f t="shared" si="0"/>
         <v>2204</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="51">
+      <c r="B28" s="38">
         <v>240</v>
       </c>
-      <c r="C28" s="47"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="44">
+      <c r="H28" s="28"/>
+      <c r="I28" s="31">
         <f t="shared" si="0"/>
         <v>2278</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="51">
+      <c r="B29" s="38">
         <v>250</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="44">
+      <c r="H29" s="28"/>
+      <c r="I29" s="31">
         <f t="shared" si="0"/>
         <v>2352</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="51">
+      <c r="B30" s="38">
         <v>260</v>
       </c>
-      <c r="C30" s="47"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="44">
+      <c r="H30" s="28"/>
+      <c r="I30" s="31">
         <f t="shared" si="0"/>
         <v>2426</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="53">
+      <c r="B31" s="40">
         <v>270</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="45">
+      <c r="C31" s="36"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="32">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1725,7 +1725,7 @@
   <dimension ref="B1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:N7"/>
+      <selection activeCell="G4" sqref="G4:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,24 +1749,24 @@
       </c>
       <c r="C3" s="7" t="str">
         <f>IF(ISBLANK(Tables!C4), DEC2HEX(65535), DEC2HEX(Tables!C4, 4))</f>
-        <v>0244</v>
+        <v>02EE</v>
       </c>
       <c r="D3" s="9" t="str">
         <f>MID(C3,1,2)&amp;" "&amp;MID(C3,3,2)&amp;" "</f>
-        <v xml:space="preserve">02 44 </v>
-      </c>
-      <c r="G3" s="20" t="s">
+        <v xml:space="preserve">02 EE </v>
+      </c>
+      <c r="G3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -1774,27 +1774,27 @@
       </c>
       <c r="C4" s="7" t="str">
         <f>IF(ISBLANK(Tables!C5), DEC2HEX(65535), DEC2HEX(Tables!C5, 4))</f>
-        <v>0299</v>
+        <v>033E</v>
       </c>
       <c r="D4" s="9" t="str">
         <f t="shared" ref="D4:D30" si="0">MID(C4,1,2)&amp;" "&amp;MID(C4,3,2)&amp;" "</f>
-        <v xml:space="preserve">02 99 </v>
-      </c>
-      <c r="F4" s="19" t="str">
+        <v xml:space="preserve">03 3E </v>
+      </c>
+      <c r="F4" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3)) + 0, 4)</f>
         <v>0108</v>
       </c>
-      <c r="G4" s="17" t="str">
+      <c r="G4" s="46" t="str">
         <f>F4&amp;":                           "&amp;D3&amp;D4&amp;" "&amp;D5&amp;D6</f>
-        <v xml:space="preserve">0108:                           02 44 02 99  02 EE 03 3E </v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
+        <v xml:space="preserve">0108:                           02 EE 03 3E  03 A2 03 E8 </v>
+      </c>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -1802,27 +1802,27 @@
       </c>
       <c r="C5" s="7" t="str">
         <f>IF(ISBLANK(Tables!C6), DEC2HEX(65535), DEC2HEX(Tables!C6, 4))</f>
-        <v>02EE</v>
+        <v>03A2</v>
       </c>
       <c r="D5" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">02 EE </v>
-      </c>
-      <c r="F5" s="19" t="str">
+        <v xml:space="preserve">03 A2 </v>
+      </c>
+      <c r="F5" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+8, 4)</f>
         <v>0110</v>
       </c>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="46" t="str">
         <f>F5&amp;": "&amp;D7&amp;D8&amp;" "&amp;D9&amp;D10&amp;" "&amp;D11&amp;D12&amp;" "&amp;D13&amp;D14</f>
-        <v xml:space="preserve">0110: 03 93 03 DE  04 2E 04 88  04 E2 05 46  05 AA 06 04 </v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+        <v xml:space="preserve">0110: 04 38 04 9C  04 E2 05 32  05 8C 05 E6  06 40 06 9A </v>
+      </c>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -1830,27 +1830,27 @@
       </c>
       <c r="C6" s="7" t="str">
         <f>IF(ISBLANK(Tables!C7), DEC2HEX(65535), DEC2HEX(Tables!C7, 4))</f>
-        <v>033E</v>
+        <v>03E8</v>
       </c>
       <c r="D6" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">03 3E </v>
-      </c>
-      <c r="F6" s="19" t="str">
+        <v xml:space="preserve">03 E8 </v>
+      </c>
+      <c r="F6" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+24, 4)</f>
         <v>0120</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="46" t="str">
         <f>F6&amp;": "&amp;D15&amp;D16&amp;" "&amp;D17&amp;D18&amp;" "&amp;D19&amp;D20&amp;" "&amp;D21&amp;D22</f>
-        <v xml:space="preserve">0120: 06 68 06 CC  07 26 07 80  07 DA 08 39  08 98 FF FF </v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+        <v xml:space="preserve">0120: 06 F4 07 4E  07 A8 08 02  08 52 08 A2  09 10 FF FF </v>
+      </c>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
@@ -1858,27 +1858,27 @@
       </c>
       <c r="C7" s="7" t="str">
         <f>IF(ISBLANK(Tables!C8), DEC2HEX(65535), DEC2HEX(Tables!C8, 4))</f>
-        <v>0393</v>
+        <v>0438</v>
       </c>
       <c r="D7" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">03 93 </v>
-      </c>
-      <c r="F7" s="19" t="str">
+        <v xml:space="preserve">04 38 </v>
+      </c>
+      <c r="F7" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+40, 4)</f>
         <v>0130</v>
       </c>
-      <c r="G7" s="18" t="str">
+      <c r="G7" s="49" t="str">
         <f>F7&amp;": "&amp;D23&amp;D24&amp;" "&amp;D25&amp;D26&amp;" "&amp;D27&amp;D28&amp;" "&amp;D29&amp;D30</f>
         <v xml:space="preserve">0130: FF FF FF FF  FF FF FF FF  FF FF FF FF  FF FF FF FF </v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -1886,11 +1886,11 @@
       </c>
       <c r="C8" s="7" t="str">
         <f>IF(ISBLANK(Tables!C9), DEC2HEX(65535), DEC2HEX(Tables!C9, 4))</f>
-        <v>03DE</v>
+        <v>049C</v>
       </c>
       <c r="D8" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">03 DE </v>
+        <v xml:space="preserve">04 9C </v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -1900,11 +1900,11 @@
       </c>
       <c r="C9" s="7" t="str">
         <f>IF(ISBLANK(Tables!C10), DEC2HEX(65535), DEC2HEX(Tables!C10, 4))</f>
-        <v>042E</v>
+        <v>04E2</v>
       </c>
       <c r="D9" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">04 2E </v>
+        <v xml:space="preserve">04 E2 </v>
       </c>
       <c r="F9" s="10"/>
     </row>
@@ -1914,11 +1914,11 @@
       </c>
       <c r="C10" s="7" t="str">
         <f>IF(ISBLANK(Tables!C11), DEC2HEX(65535), DEC2HEX(Tables!C11, 4))</f>
-        <v>0488</v>
+        <v>0532</v>
       </c>
       <c r="D10" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">04 88 </v>
+        <v xml:space="preserve">05 32 </v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -1928,11 +1928,11 @@
       </c>
       <c r="C11" s="7" t="str">
         <f>IF(ISBLANK(Tables!C12), DEC2HEX(65535), DEC2HEX(Tables!C12, 4))</f>
-        <v>04E2</v>
+        <v>058C</v>
       </c>
       <c r="D11" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">04 E2 </v>
+        <v xml:space="preserve">05 8C </v>
       </c>
       <c r="F11" s="10"/>
     </row>
@@ -1942,11 +1942,11 @@
       </c>
       <c r="C12" s="7" t="str">
         <f>IF(ISBLANK(Tables!C13), DEC2HEX(65535), DEC2HEX(Tables!C13, 4))</f>
-        <v>0546</v>
+        <v>05E6</v>
       </c>
       <c r="D12" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">05 46 </v>
+        <v xml:space="preserve">05 E6 </v>
       </c>
       <c r="F12" s="10"/>
     </row>
@@ -1956,11 +1956,11 @@
       </c>
       <c r="C13" s="7" t="str">
         <f>IF(ISBLANK(Tables!C14), DEC2HEX(65535), DEC2HEX(Tables!C14, 4))</f>
-        <v>05AA</v>
+        <v>0640</v>
       </c>
       <c r="D13" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">05 AA </v>
+        <v xml:space="preserve">06 40 </v>
       </c>
       <c r="F13" s="10"/>
     </row>
@@ -1970,11 +1970,11 @@
       </c>
       <c r="C14" s="7" t="str">
         <f>IF(ISBLANK(Tables!C15), DEC2HEX(65535), DEC2HEX(Tables!C15, 4))</f>
-        <v>0604</v>
+        <v>069A</v>
       </c>
       <c r="D14" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">06 04 </v>
+        <v xml:space="preserve">06 9A </v>
       </c>
       <c r="F14" s="10"/>
     </row>
@@ -1984,11 +1984,11 @@
       </c>
       <c r="C15" s="7" t="str">
         <f>IF(ISBLANK(Tables!C16), DEC2HEX(65535), DEC2HEX(Tables!C16, 4))</f>
-        <v>0668</v>
+        <v>06F4</v>
       </c>
       <c r="D15" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">06 68 </v>
+        <v xml:space="preserve">06 F4 </v>
       </c>
       <c r="F15" s="10"/>
     </row>
@@ -1998,11 +1998,11 @@
       </c>
       <c r="C16" s="7" t="str">
         <f>IF(ISBLANK(Tables!C17), DEC2HEX(65535), DEC2HEX(Tables!C17, 4))</f>
-        <v>06CC</v>
+        <v>074E</v>
       </c>
       <c r="D16" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">06 CC </v>
+        <v xml:space="preserve">07 4E </v>
       </c>
       <c r="F16" s="10"/>
     </row>
@@ -2012,11 +2012,11 @@
       </c>
       <c r="C17" s="7" t="str">
         <f>IF(ISBLANK(Tables!C18), DEC2HEX(65535), DEC2HEX(Tables!C18, 4))</f>
-        <v>0726</v>
+        <v>07A8</v>
       </c>
       <c r="D17" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">07 26 </v>
+        <v xml:space="preserve">07 A8 </v>
       </c>
       <c r="F17" s="10"/>
     </row>
@@ -2026,11 +2026,11 @@
       </c>
       <c r="C18" s="7" t="str">
         <f>IF(ISBLANK(Tables!C19), DEC2HEX(65535), DEC2HEX(Tables!C19, 4))</f>
-        <v>0780</v>
+        <v>0802</v>
       </c>
       <c r="D18" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">07 80 </v>
+        <v xml:space="preserve">08 02 </v>
       </c>
       <c r="F18" s="10"/>
     </row>
@@ -2040,11 +2040,11 @@
       </c>
       <c r="C19" s="7" t="str">
         <f>IF(ISBLANK(Tables!C20), DEC2HEX(65535), DEC2HEX(Tables!C20, 4))</f>
-        <v>07DA</v>
+        <v>0852</v>
       </c>
       <c r="D19" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">07 DA </v>
+        <v xml:space="preserve">08 52 </v>
       </c>
       <c r="F19" s="10"/>
     </row>
@@ -2054,11 +2054,11 @@
       </c>
       <c r="C20" s="7" t="str">
         <f>IF(ISBLANK(Tables!C21), DEC2HEX(65535), DEC2HEX(Tables!C21, 4))</f>
-        <v>0839</v>
+        <v>08A2</v>
       </c>
       <c r="D20" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">08 39 </v>
+        <v xml:space="preserve">08 A2 </v>
       </c>
       <c r="F20" s="10"/>
     </row>
@@ -2068,11 +2068,11 @@
       </c>
       <c r="C21" s="7" t="str">
         <f>IF(ISBLANK(Tables!C22), DEC2HEX(65535), DEC2HEX(Tables!C22, 4))</f>
-        <v>0898</v>
+        <v>0910</v>
       </c>
       <c r="D21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">08 98 </v>
+        <v xml:space="preserve">09 10 </v>
       </c>
       <c r="F21" s="10"/>
     </row>
@@ -2242,18 +2242,18 @@
         <f>MID(C3,1,2)&amp;" "&amp;MID(C3,3,2)&amp;" "</f>
         <v xml:space="preserve">02 80 </v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -2267,21 +2267,21 @@
         <f t="shared" ref="D4:D30" si="0">MID(C4,1,2)&amp;" "&amp;MID(C4,3,2)&amp;" "</f>
         <v xml:space="preserve">02 DA </v>
       </c>
-      <c r="F4" s="19" t="str">
+      <c r="F4" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3)) + 0, 4)</f>
         <v>01C8</v>
       </c>
-      <c r="G4" s="17" t="str">
+      <c r="G4" s="46" t="str">
         <f>F4&amp;":                           "&amp;D3&amp;D4&amp;" "&amp;D5&amp;D6</f>
         <v xml:space="preserve">01C8:                           02 80 02 DA  03 20 03 7A </v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -2295,21 +2295,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 20 </v>
       </c>
-      <c r="F5" s="19" t="str">
+      <c r="F5" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+8, 4)</f>
         <v>01D0</v>
       </c>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="46" t="str">
         <f>F5&amp;": "&amp;D7&amp;D8&amp;" "&amp;D9&amp;D10&amp;" "&amp;D11&amp;D12&amp;" "&amp;D13&amp;D14</f>
         <v xml:space="preserve">01D0: 03 D9 04 2E  04 7E 04 E2  05 3C 05 96  05 FA 06 54 </v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -2323,21 +2323,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 7A </v>
       </c>
-      <c r="F6" s="19" t="str">
+      <c r="F6" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+24, 4)</f>
         <v>01E0</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="46" t="str">
         <f>F6&amp;": "&amp;D15&amp;D16&amp;" "&amp;D17&amp;D18&amp;" "&amp;D19&amp;D20&amp;" "&amp;D21&amp;D22</f>
         <v xml:space="preserve">01E0: 06 AE 07 08  07 6C 07 C6  08 20 08 7A  08 D4 FF FF </v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
@@ -2351,21 +2351,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 D9 </v>
       </c>
-      <c r="F7" s="19" t="str">
+      <c r="F7" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+40, 4)</f>
         <v>01F0</v>
       </c>
-      <c r="G7" s="18" t="str">
+      <c r="G7" s="49" t="str">
         <f>F7&amp;": "&amp;D23&amp;D24&amp;" "&amp;D25&amp;D26&amp;" "&amp;D27&amp;D28&amp;" "&amp;D29&amp;D30</f>
         <v xml:space="preserve">01F0: FF FF FF FF  FF FF FF FF  FF FF FF FF  FF FF FF FF </v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -2729,18 +2729,18 @@
         <f>MID(C3,1,2)&amp;" "&amp;MID(C3,3,2)&amp;" "</f>
         <v xml:space="preserve">02 62 </v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -2754,21 +2754,21 @@
         <f t="shared" ref="D4:D30" si="0">MID(C4,1,2)&amp;" "&amp;MID(C4,3,2)&amp;" "</f>
         <v xml:space="preserve">02 AD </v>
       </c>
-      <c r="F4" s="19" t="str">
+      <c r="F4" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3)) + 0, 4)</f>
         <v>0288</v>
       </c>
-      <c r="G4" s="17" t="str">
+      <c r="G4" s="46" t="str">
         <f>F4&amp;":                           "&amp;D3&amp;D4&amp;" "&amp;D5&amp;D6</f>
         <v xml:space="preserve">0288:                           02 62 02 AD  02 EE 03 3E </v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -2782,21 +2782,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">02 EE </v>
       </c>
-      <c r="F5" s="19" t="str">
+      <c r="F5" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+8, 4)</f>
         <v>0290</v>
       </c>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="46" t="str">
         <f>F5&amp;": "&amp;D7&amp;D8&amp;" "&amp;D9&amp;D10&amp;" "&amp;D11&amp;D12&amp;" "&amp;D13&amp;D14</f>
         <v xml:space="preserve">0290: 03 93 04 2E  04 38 04 88  04 E2 05 32  05 82 05 E6 </v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -2810,21 +2810,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 3E </v>
       </c>
-      <c r="F6" s="19" t="str">
+      <c r="F6" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+24, 4)</f>
         <v>02A0</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="46" t="str">
         <f>F6&amp;": "&amp;D15&amp;D16&amp;" "&amp;D17&amp;D18&amp;" "&amp;D19&amp;D20&amp;" "&amp;D21&amp;D22</f>
         <v xml:space="preserve">02A0: 06 22 06 72  06 D6 07 26  07 85 07 DA  08 39 FF FF </v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
@@ -2838,21 +2838,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 93 </v>
       </c>
-      <c r="F7" s="19" t="str">
+      <c r="F7" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+40, 4)</f>
         <v>02B0</v>
       </c>
-      <c r="G7" s="18" t="str">
+      <c r="G7" s="49" t="str">
         <f>F7&amp;": "&amp;D23&amp;D24&amp;" "&amp;D25&amp;D26&amp;" "&amp;D27&amp;D28&amp;" "&amp;D29&amp;D30</f>
         <v xml:space="preserve">02B0: FF FF FF FF  FF FF FF FF  FF FF FF FF  FF FF FF FF </v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -3216,18 +3216,18 @@
         <f>MID(C3,1,2)&amp;" "&amp;MID(C3,3,2)&amp;" "</f>
         <v xml:space="preserve">02 44 </v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -3241,21 +3241,21 @@
         <f t="shared" ref="D4:D30" si="0">MID(C4,1,2)&amp;" "&amp;MID(C4,3,2)&amp;" "</f>
         <v xml:space="preserve">02 94 </v>
       </c>
-      <c r="F4" s="19" t="str">
+      <c r="F4" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3)) + 0, 4)</f>
         <v>0348</v>
       </c>
-      <c r="G4" s="17" t="str">
+      <c r="G4" s="46" t="str">
         <f>F4&amp;":                           "&amp;D3&amp;D4&amp;" "&amp;D5&amp;D6</f>
         <v xml:space="preserve">0348:                           02 44 02 94  02 E4 03 34 </v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -3269,21 +3269,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">02 E4 </v>
       </c>
-      <c r="F5" s="19" t="str">
+      <c r="F5" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+8, 4)</f>
         <v>0350</v>
       </c>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="46" t="str">
         <f>F5&amp;": "&amp;D7&amp;D8&amp;" "&amp;D9&amp;D10&amp;" "&amp;D11&amp;D12&amp;" "&amp;D13&amp;D14</f>
         <v xml:space="preserve">0350: 03 93 03 DE  04 4C 04 9C  04 F6 05 50  05 A0 05 FA </v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -3297,21 +3297,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 34 </v>
       </c>
-      <c r="F6" s="19" t="str">
+      <c r="F6" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+24, 4)</f>
         <v>0360</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="46" t="str">
         <f>F6&amp;": "&amp;D15&amp;D16&amp;" "&amp;D17&amp;D18&amp;" "&amp;D19&amp;D20&amp;" "&amp;D21&amp;D22</f>
         <v xml:space="preserve">0360: 06 5E 06 C2  07 1C 07 76  07 DA 08 34  08 7A FF FF </v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
@@ -3325,21 +3325,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 93 </v>
       </c>
-      <c r="F7" s="19" t="str">
+      <c r="F7" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+40, 4)</f>
         <v>0370</v>
       </c>
-      <c r="G7" s="18" t="str">
+      <c r="G7" s="49" t="str">
         <f>F7&amp;": "&amp;D23&amp;D24&amp;" "&amp;D25&amp;D26&amp;" "&amp;D27&amp;D28&amp;" "&amp;D29&amp;D30</f>
         <v xml:space="preserve">0370: FF FF FF FF  FF FF FF FF  FF FF FF FF  FF FF FF FF </v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -3703,18 +3703,18 @@
         <f>MID(C3,1,2)&amp;" "&amp;MID(C3,3,2)&amp;" "</f>
         <v xml:space="preserve">02 62 </v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -3728,21 +3728,21 @@
         <f t="shared" ref="D4:D30" si="0">MID(C4,1,2)&amp;" "&amp;MID(C4,3,2)&amp;" "</f>
         <v xml:space="preserve">02 A8 </v>
       </c>
-      <c r="F4" s="19" t="str">
+      <c r="F4" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3)) + 0, 4)</f>
         <v>0408</v>
       </c>
-      <c r="G4" s="17" t="str">
+      <c r="G4" s="46" t="str">
         <f>F4&amp;":                           "&amp;D3&amp;D4&amp;" "&amp;D5&amp;D6</f>
         <v xml:space="preserve">0408:                           02 62 02 A8  02 EE 03 3E </v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -3756,21 +3756,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">02 EE </v>
       </c>
-      <c r="F5" s="19" t="str">
+      <c r="F5" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+8, 4)</f>
         <v>0410</v>
       </c>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="46" t="str">
         <f>F5&amp;": "&amp;D7&amp;D8&amp;" "&amp;D9&amp;D10&amp;" "&amp;D11&amp;D12&amp;" "&amp;D13&amp;D14</f>
         <v xml:space="preserve">0410: 03 8E 03 DE  04 2E 04 88  04 D8 05 28  05 78 05 C8 </v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -3784,21 +3784,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 3E </v>
       </c>
-      <c r="F6" s="19" t="str">
+      <c r="F6" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+24, 4)</f>
         <v>0420</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="46" t="str">
         <f>F6&amp;": "&amp;D15&amp;D16&amp;" "&amp;D17&amp;D18&amp;" "&amp;D19&amp;D20&amp;" "&amp;D21&amp;D22</f>
         <v xml:space="preserve">0420: 06 18 06 68  06 B8 07 08  07 6C 07 B2  08 16 FF FF </v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
@@ -3812,21 +3812,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 8E </v>
       </c>
-      <c r="F7" s="19" t="str">
+      <c r="F7" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+40, 4)</f>
         <v>0430</v>
       </c>
-      <c r="G7" s="18" t="str">
+      <c r="G7" s="49" t="str">
         <f>F7&amp;": "&amp;D23&amp;D24&amp;" "&amp;D25&amp;D26&amp;" "&amp;D27&amp;D28&amp;" "&amp;D29&amp;D30</f>
         <v xml:space="preserve">0430: FF FF FF FF  FF FF FF FF  FF FF FF FF  FF FF FF FF </v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -4190,18 +4190,18 @@
         <f>MID(C3,1,2)&amp;" "&amp;MID(C3,3,2)&amp;" "</f>
         <v xml:space="preserve">02 44 </v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -4215,21 +4215,21 @@
         <f t="shared" ref="D4:D30" si="0">MID(C4,1,2)&amp;" "&amp;MID(C4,3,2)&amp;" "</f>
         <v xml:space="preserve">02 94 </v>
       </c>
-      <c r="F4" s="19" t="str">
+      <c r="F4" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3)) + 0, 4)</f>
         <v>04C8</v>
       </c>
-      <c r="G4" s="17" t="str">
+      <c r="G4" s="46" t="str">
         <f>F4&amp;":                           "&amp;D3&amp;D4&amp;" "&amp;D5&amp;D6</f>
         <v xml:space="preserve">04C8:                           02 44 02 94  02 EE 03 3E </v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -4243,21 +4243,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">02 EE </v>
       </c>
-      <c r="F5" s="19" t="str">
+      <c r="F5" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+8, 4)</f>
         <v>04D0</v>
       </c>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="46" t="str">
         <f>F5&amp;": "&amp;D7&amp;D8&amp;" "&amp;D9&amp;D10&amp;" "&amp;D11&amp;D12&amp;" "&amp;D13&amp;D14</f>
         <v xml:space="preserve">04D0: 03 93 03 DE  04 2E 04 88  04 E2 05 41  05 A0 05 FA </v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -4271,21 +4271,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 3E </v>
       </c>
-      <c r="F6" s="19" t="str">
+      <c r="F6" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+24, 4)</f>
         <v>04E0</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="46" t="str">
         <f>F6&amp;": "&amp;D15&amp;D16&amp;" "&amp;D17&amp;D18&amp;" "&amp;D19&amp;D20&amp;" "&amp;D21&amp;D22</f>
         <v xml:space="preserve">04E0: 06 4A 06 9A  06 F4 07 44  07 A8 08 02  08 52 FF FF </v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
@@ -4299,21 +4299,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 93 </v>
       </c>
-      <c r="F7" s="19" t="str">
+      <c r="F7" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+40, 4)</f>
         <v>04F0</v>
       </c>
-      <c r="G7" s="18" t="str">
+      <c r="G7" s="49" t="str">
         <f>F7&amp;": "&amp;D23&amp;D24&amp;" "&amp;D25&amp;D26&amp;" "&amp;D27&amp;D28&amp;" "&amp;D29&amp;D30</f>
         <v xml:space="preserve">04F0: FF FF FF FF  FF FF FF FF  FF FF FF FF  FF FF FF FF </v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -4646,7 +4646,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -4677,18 +4677,18 @@
         <f>MID(C3,1,2)&amp;" "&amp;MID(C3,3,2)&amp;" "</f>
         <v xml:space="preserve">01 F4 </v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -4702,21 +4702,21 @@
         <f t="shared" ref="D4:D30" si="0">MID(C4,1,2)&amp;" "&amp;MID(C4,3,2)&amp;" "</f>
         <v xml:space="preserve">02 3E </v>
       </c>
-      <c r="F4" s="19" t="str">
+      <c r="F4" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3)) + 0, 4)</f>
         <v>0548</v>
       </c>
-      <c r="G4" s="17" t="str">
+      <c r="G4" s="46" t="str">
         <f>F4&amp;":                           "&amp;D3&amp;D4&amp;" "&amp;D5&amp;D6</f>
         <v xml:space="preserve">0548:                           01 F4 02 3E  02 88 02 D2 </v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -4730,21 +4730,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">02 88 </v>
       </c>
-      <c r="F5" s="19" t="str">
+      <c r="F5" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+8, 4)</f>
         <v>0550</v>
       </c>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="46" t="str">
         <f>F5&amp;": "&amp;D7&amp;D8&amp;" "&amp;D9&amp;D10&amp;" "&amp;D11&amp;D12&amp;" "&amp;D13&amp;D14</f>
         <v xml:space="preserve">0550: 03 1C 03 66  03 B0 03 FB  04 45 04 8F  04 D9 05 23 </v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -4758,21 +4758,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">02 D2 </v>
       </c>
-      <c r="F6" s="19" t="str">
+      <c r="F6" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+24, 4)</f>
         <v>0560</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="46" t="str">
         <f>F6&amp;": "&amp;D15&amp;D16&amp;" "&amp;D17&amp;D18&amp;" "&amp;D19&amp;D20&amp;" "&amp;D21&amp;D22</f>
         <v xml:space="preserve">0560: 05 6D 05 B7  06 01 06 4B  06 95 06 DF  07 29 07 73 </v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
@@ -4786,21 +4786,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">03 1C </v>
       </c>
-      <c r="F7" s="19" t="str">
+      <c r="F7" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+40, 4)</f>
         <v>0570</v>
       </c>
-      <c r="G7" s="18" t="str">
+      <c r="G7" s="49" t="str">
         <f>F7&amp;": "&amp;D23&amp;D24&amp;" "&amp;D25&amp;D26&amp;" "&amp;D27&amp;D28&amp;" "&amp;D29&amp;D30</f>
         <v xml:space="preserve">0570: 07 BD 08 08  08 52 08 9C  08 E6 09 30  09 7A 09 C4 </v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="4">

</xml_diff>